<commit_message>
fixed some alignments for RAPTOR
</commit_message>
<xml_diff>
--- a/seq/RAxML_run_summary.xlsx
+++ b/seq/RAxML_run_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollo\Documents\Box Sync\EEOB563\EEOB563_S19FinalProject\seq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6F7E1-6D26-4837-B4FF-C6FB417E39B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF353990-18BC-475C-AD4F-BD1C46B02040}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="1340" windowWidth="18070" windowHeight="6440" xr2:uid="{3A8E787D-85F8-4AF4-B4A9-9C09B004D04D}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>RaxML_7</t>
   </si>
   <si>
-    <t>RaxML_8</t>
-  </si>
-  <si>
     <t>RaxML_9</t>
   </si>
   <si>
@@ -132,18 +129,12 @@
     <t>RaxML__12</t>
   </si>
   <si>
-    <t>RaxML__13</t>
-  </si>
-  <si>
     <t>RAPTORB_NCBI_HomoloGene.fasta</t>
   </si>
   <si>
     <t>RaxML____15</t>
   </si>
   <si>
-    <t>RaxML____16</t>
-  </si>
-  <si>
     <t>RaxML_____16</t>
   </si>
   <si>
@@ -186,7 +177,16 @@
     <t>RaxML__14</t>
   </si>
   <si>
-    <t>RaxML__________20</t>
+    <t>RaxML__________19</t>
+  </si>
+  <si>
+    <t>RaxML___________20</t>
+  </si>
+  <si>
+    <t>RaxML____________22</t>
+  </si>
+  <si>
+    <t>RaxML_____________23</t>
   </si>
 </sst>
 </file>
@@ -234,10 +234,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -555,13 +554,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F246AD-F8A7-4AB0-8D93-D301BD698F09}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.90625" customWidth="1"/>
@@ -583,268 +582,268 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-13153.313185999999</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-13017.26355</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-4911.59584</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-4809.521189</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-5415.7299329999996</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-5363.3064430000004</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3">
-        <v>-13153.313185999999</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-29500.945144000001</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-13017.26355</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3">
-        <v>-4911.59584</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3">
-        <v>-4809.521189</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-5415.7299329999996</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3">
-        <v>-5363.3064430000004</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3">
-        <v>-29500.945144000001</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
         <v>-29368.363826000001</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2">
+        <v>-99416.866563000003</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3">
-        <v>-99416.866563000003</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2">
         <v>-91416.032231000005</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
         <v>-29567.364072</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
         <v>-28995.531053999999</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>16</v>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -852,19 +851,19 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <v>-65706.702879999997</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -872,19 +871,19 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>-64440.917826999997</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -892,255 +891,255 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>-64172.153708999998</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1">
         <v>-31810.059519999999</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1">
         <v>-31479.332747</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1">
         <v>-72124.902675000005</v>
       </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21">
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1">
         <v>-70926.891969000004</v>
       </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23">
         <v>-116832.449767</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2">
+        <v>-38203.595950000003</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2">
+        <v>-37352.607713999998</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="3">
-        <v>-38203.595950000003</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="2">
+        <v>-45328.390428999999</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="3">
-        <v>-37352.607713999998</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="2">
+        <v>-44673.667219000003</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="3">
-        <v>-45328.390428999999</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="3">
-        <v>-44673.667219000003</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="3">
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2">
         <v>-118676.162627</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>16</v>
+      <c r="E28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>